<commit_message>
Update ml-data matrix with two new reqts
</commit_message>
<xml_diff>
--- a/docs/figures/tables.xlsx
+++ b/docs/figures/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\smirk\docs\figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\smirk\docs\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72179834-32F1-4F9C-8D0B-DC09AFC5825A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1395E4-DD7A-42C9-BFC2-9D343335BF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28320" yWindow="330" windowWidth="27495" windowHeight="20940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data-Matrix" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="50">
   <si>
     <t>SYS-ML-REQ1</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>SYS-ROB-REQ3</t>
+  </si>
+  <si>
+    <t>SYS-ROB-REQ4</t>
   </si>
 </sst>
 </file>
@@ -289,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -311,6 +317,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -325,12 +340,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -621,71 +630,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85438ABE-8CC5-41BE-881E-8B0C27850710}">
-  <dimension ref="B2:Y14"/>
+  <dimension ref="B2:Y16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="5.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="21" width="5.6640625" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="5.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="21" width="5.7109375" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:25" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="14" t="s">
+    <row r="2" spans="2:25" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-    </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="E3" s="15" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15" t="s">
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15" t="s">
+      <c r="R3" s="11"/>
+      <c r="S3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-    </row>
-    <row r="4" spans="2:25" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+    </row>
+    <row r="4" spans="2:25" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="3"/>
       <c r="E4" s="6" t="s">
         <v>9</v>
@@ -743,11 +752,11 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
     </row>
-    <row r="5" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="13" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -803,9 +812,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
+    <row r="6" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="5" t="s">
         <v>1</v>
       </c>
@@ -835,9 +844,9 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10" t="s">
+    <row r="7" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -867,9 +876,9 @@
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
     </row>
-    <row r="8" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
+    <row r="8" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="5" t="s">
         <v>3</v>
       </c>
@@ -893,9 +902,9 @@
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
     </row>
-    <row r="9" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
+    <row r="9" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="5" t="s">
         <v>4</v>
       </c>
@@ -927,35 +936,35 @@
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
     </row>
-    <row r="10" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
+    <row r="10" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="13"/>
-    </row>
-    <row r="11" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="16"/>
+    </row>
+    <row r="11" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="5" t="s">
         <v>6</v>
       </c>
@@ -983,35 +992,35 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
+    <row r="12" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="13"/>
-    </row>
-    <row r="13" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="10" t="s">
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="16"/>
+    </row>
+    <row r="13" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -1045,53 +1054,121 @@
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
     </row>
-    <row r="14" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
+    <row r="14" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+    </row>
+    <row r="15" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+    </row>
+    <row r="16" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B5:B16"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="E10:U10"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="E12:U12"/>
     <mergeCell ref="E2:U2"/>
     <mergeCell ref="E3:K3"/>
     <mergeCell ref="L3:P3"/>
     <mergeCell ref="Q3:R3"/>
     <mergeCell ref="S3:U3"/>
-    <mergeCell ref="B5:B14"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="E10:U10"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E12:U12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1100,57 +1177,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5BCC75-6C56-40A1-9D97-7C7874AAD5C0}">
-  <dimension ref="B2:Q14"/>
+  <dimension ref="B2:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O4:W13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="5.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="5.6640625" style="1" customWidth="1"/>
-    <col min="14" max="16" width="9.109375" style="1"/>
-    <col min="17" max="17" width="16.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.33203125" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="5.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="5.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="16.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="14" t="s">
+    <row r="2" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E3" s="15" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="E3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16" t="s">
+      <c r="H3" s="11"/>
+      <c r="I3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="18"/>
-    </row>
-    <row r="4" spans="2:17" ht="196.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="19"/>
+    </row>
+    <row r="4" spans="2:17" ht="196.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="3"/>
       <c r="E4" s="6" t="s">
         <v>39</v>
@@ -1176,11 +1253,11 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="13" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -1202,9 +1279,9 @@
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
+    <row r="6" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="5" t="s">
         <v>1</v>
       </c>
@@ -1218,9 +1295,9 @@
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10" t="s">
+    <row r="7" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1236,9 +1313,9 @@
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
+    <row r="8" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="5" t="s">
         <v>3</v>
       </c>
@@ -1252,9 +1329,9 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
+    <row r="9" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="5" t="s">
         <v>4</v>
       </c>
@@ -1268,27 +1345,27 @@
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
+    <row r="10" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="13"/>
-    </row>
-    <row r="11" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="16"/>
+    </row>
+    <row r="11" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="5" t="s">
         <v>6</v>
       </c>
@@ -1302,27 +1379,27 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
+    <row r="12" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="13"/>
-    </row>
-    <row r="13" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="10" t="s">
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="16"/>
+    </row>
+    <row r="13" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -1338,34 +1415,66 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
+    <row r="14" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B5:B16"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="E10:M10"/>
+    <mergeCell ref="E12:M12"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="I3:M3"/>
     <mergeCell ref="E2:M2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B5:B14"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="E10:M10"/>
-    <mergeCell ref="E12:M12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1380,65 +1489,65 @@
       <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="5.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="21" width="5.6640625" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="5.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="21" width="5.7109375" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:25" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="14" t="s">
+    <row r="2" spans="2:25" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-    </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="E3" s="15" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15" t="s">
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15" t="s">
+      <c r="R3" s="11"/>
+      <c r="S3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-    </row>
-    <row r="4" spans="2:25" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+    </row>
+    <row r="4" spans="2:25" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="3"/>
       <c r="E4" s="6" t="s">
         <v>9</v>
@@ -1496,11 +1605,11 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
     </row>
-    <row r="5" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="13" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -1524,9 +1633,9 @@
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
     </row>
-    <row r="6" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
+    <row r="6" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="5" t="s">
         <v>1</v>
       </c>
@@ -1548,9 +1657,9 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10" t="s">
+    <row r="7" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1574,9 +1683,9 @@
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
     </row>
-    <row r="8" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
+    <row r="8" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="5" t="s">
         <v>3</v>
       </c>
@@ -1598,9 +1707,9 @@
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
     </row>
-    <row r="9" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
+    <row r="9" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="5" t="s">
         <v>4</v>
       </c>
@@ -1622,9 +1731,9 @@
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
     </row>
-    <row r="10" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
+    <row r="10" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1646,9 +1755,9 @@
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
     </row>
-    <row r="11" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
+    <row r="11" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="5" t="s">
         <v>6</v>
       </c>
@@ -1670,9 +1779,9 @@
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
     </row>
-    <row r="12" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10" t="s">
+    <row r="12" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -1696,9 +1805,9 @@
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
     </row>
-    <row r="13" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
+    <row r="13" spans="2:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="5" t="s">
         <v>8</v>
       </c>

</xml_diff>